<commit_message>
Cambio de backlog v1
</commit_message>
<xml_diff>
--- a/Documentacion/Product_Backlog.xlsx
+++ b/Documentacion/Product_Backlog.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESPOCH\Octavo Semestre\Aplicaciones Informáticas II\Proyecto Inglés\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_ProyectoApps2\App_ingles_v5\English\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A05CB2D-CB3A-4075-9922-D778DBA0FD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DBEC46-E958-440C-A620-75645473011D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$A$1:$I$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$A$1:$I$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
   <si>
     <t>Identificador (ID) de la Historia</t>
   </si>
@@ -363,6 +363,12 @@
   </si>
   <si>
     <t>Baja</t>
+  </si>
+  <si>
+    <t>Revisión de la Capa de Acceso a Datos</t>
+  </si>
+  <si>
+    <t>Elaboración de los diagramas de procesos</t>
   </si>
 </sst>
 </file>
@@ -1111,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I26"/>
+  <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="87" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="87" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1297,7 +1303,7 @@
         <v>72</v>
       </c>
       <c r="F9" s="27">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="G9" s="28" t="s">
         <v>77</v>
@@ -1310,246 +1316,246 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="27">
+        <v>50</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="27">
+        <v>50</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="27">
-        <v>160</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="14" t="s">
+      <c r="E12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="27">
+        <v>110</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="30">
-        <v>20</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="12">
-        <v>40</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="15" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="18">
-        <v>30</v>
-      </c>
-      <c r="G13" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="30">
+        <v>20</v>
+      </c>
+      <c r="G13" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="16" t="s">
         <v>20</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>66</v>
+      <c r="B14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="18">
-        <v>70</v>
+      <c r="F14" s="12">
+        <v>40</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="19"/>
+      <c r="H14" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="I14" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>72</v>
       </c>
       <c r="F15" s="18">
-        <v>80</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>80</v>
+        <v>30</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>79</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="15" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>72</v>
       </c>
       <c r="F16" s="18">
-        <v>80</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>20</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>72</v>
       </c>
       <c r="F17" s="18">
-        <v>160</v>
-      </c>
-      <c r="G17" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>80</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>20</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>72</v>
       </c>
       <c r="F18" s="18">
-        <v>160</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>80</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>72</v>
@@ -1557,77 +1563,77 @@
       <c r="F19" s="18">
         <v>160</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="18">
+        <v>160</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="18">
+        <v>160</v>
+      </c>
+      <c r="G21" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="14" t="s">
+      <c r="H21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="14" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="18">
-        <v>30</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="18">
-        <v>100</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>72</v>
@@ -1642,7 +1648,7 @@
         <v>20</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1650,19 +1656,19 @@
         <v>42</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>72</v>
       </c>
       <c r="F23" s="18">
-        <v>160</v>
-      </c>
-      <c r="G23" s="38" t="s">
-        <v>85</v>
+        <v>100</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>84</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>20</v>
@@ -1672,80 +1678,132 @@
       </c>
     </row>
     <row r="24" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="18">
+        <v>30</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="18">
+        <v>160</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="12">
-        <v>30</v>
-      </c>
-      <c r="G24" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="12">
-        <v>100</v>
-      </c>
-      <c r="G25" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="E26" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="12">
         <v>30</v>
       </c>
       <c r="G26" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="12">
+        <v>100</v>
+      </c>
+      <c r="G27" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="40">
+        <v>30</v>
+      </c>
+      <c r="G28" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I28" s="14" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>